<commit_message>
Inline Test Block and Pre-Req
Pre-req for module running; Test block commented with a print('Test Block') to track when debug code is active.
</commit_message>
<xml_diff>
--- a/Measures.xlsx
+++ b/Measures.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpremo\OneDrive\Python\Spotter-Amrron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\OneDrive\Python\Spotter-Amrron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{6EDC02F7-4C90-483A-B6D2-C9F823378731}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CD589B43-9149-41CA-9F3A-6C0BEC6C2E00}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F94C4AE-E8C6-4C71-8566-F2DABD92D882}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" xr2:uid="{3B2BA4DA-ED28-442C-94E4-7266A9A05D73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{3B2BA4DA-ED28-442C-94E4-7266A9A05D73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datastore" sheetId="1" r:id="rId1"/>
+    <sheet name="Output Message" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="130">
   <si>
     <t>Data Element</t>
   </si>
@@ -143,9 +145,6 @@
     <t>% Increase</t>
   </si>
   <si>
-    <t>PST</t>
-  </si>
-  <si>
     <t>PDT</t>
   </si>
   <si>
@@ -318,13 +317,151 @@
   </si>
   <si>
     <t>Interval</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Viewer (PyPortal ; M5Stack)</t>
+  </si>
+  <si>
+    <t>Adafruit.io</t>
+  </si>
+  <si>
+    <t>DataIO</t>
+  </si>
+  <si>
+    <t>AWS Web</t>
+  </si>
+  <si>
+    <t>AWS Greengrass</t>
+  </si>
+  <si>
+    <t>Base FLMsg (Amrronv4)</t>
+  </si>
+  <si>
+    <t>APRS</t>
+  </si>
+  <si>
+    <t>Amazon Web</t>
+  </si>
+  <si>
+    <t>AWS greengrass</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>Precedence</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Time &amp; Duration</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>FlMsg v3 Spot</t>
+  </si>
+  <si>
+    <t>FlMsg v3 Sitrep</t>
+  </si>
+  <si>
+    <t>Current YYYYMMDD-HHMMZ</t>
+  </si>
+  <si>
+    <t>Expiration YYYYMMDD-HHMMZ</t>
+  </si>
+  <si>
+    <r>
+      <t>Location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Lat/Lon, Grid Square, City)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Incident Number:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (ST-SFX-###)</t>
+    </r>
+  </si>
+  <si>
+    <t>Incident Status</t>
+  </si>
+  <si>
+    <t>Size and Scope</t>
+  </si>
+  <si>
+    <t>Overall Hazard:</t>
+  </si>
+  <si>
+    <t>Current Weather</t>
+  </si>
+  <si>
+    <t>48 hr Weather:</t>
+  </si>
+  <si>
+    <t>Infrastructure:</t>
+  </si>
+  <si>
+    <t>Political:</t>
+  </si>
+  <si>
+    <t>Civil:</t>
+  </si>
+  <si>
+    <t>Communications:</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Current UTC</t>
+  </si>
+  <si>
+    <t>Current Local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +484,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,13 +542,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,29 +877,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B177603C-F232-40E2-A2EC-0009B5C24689}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C87" sqref="C71:C87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.90625" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
@@ -739,42 +911,60 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -795,25 +985,31 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="str">
-        <f t="shared" ref="F3:F56" si="0">CONCATENATE(C3,D3,E3)</f>
+        <f t="shared" ref="F3:F55" si="0">CONCATENATE(C3,D3,E3)</f>
         <v>Wind Speed-Average</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -826,19 +1022,25 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -857,19 +1059,25 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="str">
@@ -882,19 +1090,25 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="str">
@@ -909,19 +1123,25 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>31</v>
@@ -940,19 +1160,25 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>32</v>
@@ -969,19 +1195,25 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -998,19 +1230,25 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
@@ -1027,19 +1265,25 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>32</v>
@@ -1056,19 +1300,25 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
@@ -1085,19 +1335,25 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>31</v>
@@ -1116,19 +1372,25 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>32</v>
@@ -1145,19 +1407,25 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>33</v>
@@ -1174,19 +1442,25 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>31</v>
@@ -1203,19 +1477,25 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>32</v>
@@ -1232,19 +1512,25 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>33</v>
@@ -1261,19 +1547,25 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>36</v>
@@ -1290,19 +1582,25 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="str">
@@ -1317,19 +1615,25 @@
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="str">
@@ -1342,19 +1646,25 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="str">
@@ -1367,19 +1677,25 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="str">
@@ -1392,19 +1708,25 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="str">
@@ -1419,19 +1741,25 @@
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="str">
@@ -1446,19 +1774,25 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="str">
@@ -1473,19 +1807,25 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="str">
@@ -1500,29 +1840,35 @@
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Time-Current</v>
+        <v>Time-Current UTC</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1531,108 +1877,123 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="F29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Time-Current</v>
+        <v>Time-Current Local</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Time-Current</v>
+        <v>Event Time-Event Time</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Event Time-Event Time</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="5">
+        <v>100150200300500</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="5">
-        <v>100150200300500</v>
-      </c>
+      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1640,30 +2001,49 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Counter Per Minute (CPM)10,25,40,60,100,200</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>7</v>
@@ -1677,92 +2057,112 @@
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Counter Per Minute (CPM)10,25,40,60,100,200</v>
+        <v>Micro Sieverts per hour (uSv/hr).09,.24,.38,.56,.94,1.88</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Milli Sieverts per Year-.82,2.06,3.3,4.94,8.23,16.47</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Micro Sieverts per hour (uSv/hr).09,.24,.38,.56,.94,1.88</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Milli Sieverts per Year-.82,2.06,3.3,4.94,8.23,16.47</v>
+        <v>Protests/Riots-Last week</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Protests/Riots-Last week</v>
+        <v>Average Unemployment Trend-Up .05%</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>61</v>
@@ -1772,26 +2172,32 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Average Unemployment Trend-Up .05%</v>
+        <v>Food Supplies-Normal</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>62</v>
@@ -1801,126 +2207,156 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Food Supplies-Normal</v>
+        <v>Sewer-Normal</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Sewer-Normal</v>
+        <v>Water-Normal</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Water-Normal</v>
+        <v>Gas-Normal</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Gas-Normal</v>
+        <v>Electrical households without-Normal</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>75</v>
@@ -1929,317 +2365,383 @@
         <v>54</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Electrical households without-Normal</v>
+        <v>Electrical Outages-Normal</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f t="shared" ref="F44:F49" si="1">CONCATENATE(C44,D44,E44)</f>
+        <v>TV-Normal</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Electrical Outages-Normal</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F45" s="2" t="str">
-        <f>CONCATENATE(C45,D45,E45)</f>
-        <v>TV-Normal</v>
+        <f t="shared" si="1"/>
+        <v>Radio-Normal</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="2" t="str">
-        <f>CONCATENATE(C46,D46,E46)</f>
-        <v>Radio-Normal</v>
+        <f t="shared" si="1"/>
+        <v>XM-Normal</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F47" s="2" t="str">
-        <f>CONCATENATE(C47,D47,E47)</f>
-        <v>XM-Normal</v>
+        <f t="shared" si="1"/>
+        <v>Internet-Normal</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F48" s="2" t="str">
-        <f>CONCATENATE(C48,D48,E48)</f>
-        <v>Internet-Normal</v>
+        <f t="shared" si="1"/>
+        <v>Cellular-Normal</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F49" s="2" t="str">
-        <f>CONCATENATE(C49,D49,E49)</f>
-        <v>Cellular-Normal</v>
+        <f t="shared" si="1"/>
+        <v>Landline-Normal</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="2" t="str">
-        <f>CONCATENATE(C50,D50,E50)</f>
-        <v>Landline-Normal</v>
+        <f t="shared" si="0"/>
+        <v>Buses-Normal</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F51" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Buses-Normal</v>
+        <v>Subway-Normal</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F52" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Subway-Normal</v>
+        <v>Freeway-Normal</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F53" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Freeway-Normal</v>
+        <v>Trains-Normal</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>10</v>
@@ -2248,27 +2750,33 @@
         <v>41</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F54" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Trains-Normal</v>
+        <v>Airports-Normal</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>10</v>
@@ -2277,55 +2785,54 @@
         <v>42</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F55" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Airports-Normal</v>
+        <v>Ferrys-Normal</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Ferrys-Normal</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2337,11 +2844,19 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -2351,11 +2866,19 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="C59" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -2365,11 +2888,19 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -2379,11 +2910,19 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="C61" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -2393,11 +2932,19 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="C62" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2407,11 +2954,19 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -2421,11 +2976,19 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="C64" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -2435,12 +2998,648 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="2"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+    </row>
+    <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+    </row>
+    <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+    </row>
+    <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+    </row>
+    <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2"/>
+    </row>
+    <row r="81" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2"/>
+    </row>
+    <row r="82" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="2"/>
+    </row>
+    <row r="83" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="2"/>
+    </row>
+    <row r="84" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="2"/>
+    </row>
+    <row r="85" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="2"/>
+    </row>
+    <row r="86" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
+    </row>
+    <row r="87" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1" xr:uid="{78E2BA90-B22A-4A9B-A5BE-3A01D932843C}"/>
+    <hyperlink ref="C31" r:id="rId1" xr:uid="{78E2BA90-B22A-4A9B-A5BE-3A01D932843C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C66601F-92B0-41E4-88F1-C1E069D4B581}">
+  <dimension ref="B1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{7B035AC0-413C-458D-B6F1-3B96D3A44519}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>